<commit_message>
adding express-resource-new for route controlling
</commit_message>
<xml_diff>
--- a/api.xlsx
+++ b/api.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23515"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18700" windowHeight="21060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21080" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="API" sheetId="1" r:id="rId1"/>
@@ -24,9 +24,6 @@
     <t>GET</t>
   </si>
   <si>
-    <t>/open-menus</t>
-  </si>
-  <si>
     <t>Action</t>
   </si>
   <si>
@@ -114,42 +111,6 @@
     <t>Controller#Action</t>
   </si>
   <si>
-    <t>/open-menus/:id</t>
-  </si>
-  <si>
-    <t>/open-menus/:open_menu_id/restaurant-info</t>
-  </si>
-  <si>
-    <t>/open-menus/:open_menu_id/environment</t>
-  </si>
-  <si>
-    <t>/open-menus/:open_menu_id/menus</t>
-  </si>
-  <si>
-    <t>/open-menus/:open_menu_id/menus/:menu_id</t>
-  </si>
-  <si>
-    <t>/open-menus/:open_menu_id/menus/:menu_id/menu-groups</t>
-  </si>
-  <si>
-    <t>/open-menus/:open_menu_id/menus/:menu_id/menu-groups/:menu_group_id</t>
-  </si>
-  <si>
-    <t>/open-menus/:open_menu_id/menus/:menu_id/menu-groups/:menu_group_id/menu-items</t>
-  </si>
-  <si>
-    <t>/open-menus/:open_menu_id/menus/:menu_id/menu-groups/:menu_group_id/menu-items/:menu_item_id</t>
-  </si>
-  <si>
-    <t>/open-menus/:open_menu_id/menus/:menu_id/menu-groups/:menu_group_id/menu-items/:menu_item_id/menu-item-sizes</t>
-  </si>
-  <si>
-    <t>/open-menus/:open_menu_id/menus/:menu_id/menu-groups/:menu_group_id/menu-items/:menu_item_id/menu-item-sizes/:menu_item_size_id</t>
-  </si>
-  <si>
-    <t>environment#show</t>
-  </si>
-  <si>
     <t>environment#update</t>
   </si>
   <si>
@@ -168,43 +129,82 @@
     <t>menus#destroy</t>
   </si>
   <si>
-    <t>openMenus#index</t>
-  </si>
-  <si>
-    <t>openMenus#create</t>
-  </si>
-  <si>
-    <t>openMenus#show</t>
-  </si>
-  <si>
-    <t>openMenus#update</t>
-  </si>
-  <si>
-    <t>openMenus#destroy</t>
-  </si>
-  <si>
-    <t>restaurantInfo#show</t>
-  </si>
-  <si>
-    <t>restaurantInfo#update</t>
-  </si>
-  <si>
-    <t>menuGroups#index</t>
-  </si>
-  <si>
-    <t>menuGroups#show</t>
-  </si>
-  <si>
-    <t>menuItems:index</t>
-  </si>
-  <si>
-    <t>menuItems:show</t>
-  </si>
-  <si>
-    <t>menuItemSizes:index</t>
-  </si>
-  <si>
-    <t>menuItemSizes:show</t>
+    <t>/openmenus</t>
+  </si>
+  <si>
+    <t>/openmenus/:id</t>
+  </si>
+  <si>
+    <t>/openmenus/:open_menu_id/environment</t>
+  </si>
+  <si>
+    <t>/openmenus/:open_menu_id/menus</t>
+  </si>
+  <si>
+    <t>/openmenus/:open_menu_id/menus/:menu_id/menugroups</t>
+  </si>
+  <si>
+    <t>/openmenus/:open_menu_id/menus/:menu_id/menugroups/:menu_group_id/menuitems</t>
+  </si>
+  <si>
+    <t>/openmenus/:open_menu_id/menus/:menu_id/menugroups/:menu_group_id/menuitems/:menu_item_id/menuitemsizes</t>
+  </si>
+  <si>
+    <t>/openmenus/:open_menu_id/restaurant</t>
+  </si>
+  <si>
+    <t>openmenus#index</t>
+  </si>
+  <si>
+    <t>openmenus#create</t>
+  </si>
+  <si>
+    <t>openmenus#show</t>
+  </si>
+  <si>
+    <t>openmenus#update</t>
+  </si>
+  <si>
+    <t>openmenus#destroy</t>
+  </si>
+  <si>
+    <t>restaurants#update</t>
+  </si>
+  <si>
+    <t>restaurants#index</t>
+  </si>
+  <si>
+    <t>environments#index</t>
+  </si>
+  <si>
+    <t>menugroups#index</t>
+  </si>
+  <si>
+    <t>menugroups#show</t>
+  </si>
+  <si>
+    <t>menuitems:index</t>
+  </si>
+  <si>
+    <t>menuitems:show</t>
+  </si>
+  <si>
+    <t>menuitemsizes:index</t>
+  </si>
+  <si>
+    <t>menuitemsizes:show</t>
+  </si>
+  <si>
+    <t>/openmenus/:open_menu_id/menus/:id</t>
+  </si>
+  <si>
+    <t>/openmenus/:open_menu_id/menus/:menu_id/menugroups/:id</t>
+  </si>
+  <si>
+    <t>/openmenus/:open_menu_id/menus/:menu_id/menugroups/:menu_group_id/menuitems/:id</t>
+  </si>
+  <si>
+    <t>/openmenus/:open_menu_id/menus/:menu_id/menugroups/:menu_group_id/menuitems/:menu_item_id/menuitemsizes/:id</t>
   </si>
 </sst>
 </file>
@@ -658,34 +658,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="5.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="121.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="104.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="140.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -696,13 +694,13 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="D2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -710,16 +708,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" t="s">
         <v>4</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E3" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -730,13 +728,13 @@
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="D4" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -744,16 +742,16 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="D5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -761,16 +759,16 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="D6" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -781,13 +779,13 @@
         <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="D7" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -795,16 +793,16 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="D8" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -815,13 +813,13 @@
         <v>0</v>
       </c>
       <c r="C9" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D9" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="E9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -829,16 +827,16 @@
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D10" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="E10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -849,13 +847,13 @@
         <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D11" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="E11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -863,16 +861,16 @@
         <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D12" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="E12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -883,13 +881,13 @@
         <v>0</v>
       </c>
       <c r="C13" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="D13" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="E13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -897,16 +895,16 @@
         <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="D14" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="E14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -914,16 +912,16 @@
         <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C15" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" t="s">
         <v>35</v>
       </c>
-      <c r="D15" t="s">
-        <v>48</v>
-      </c>
       <c r="E15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -934,13 +932,13 @@
         <v>0</v>
       </c>
       <c r="C16" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D16" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -951,13 +949,13 @@
         <v>0</v>
       </c>
       <c r="C17" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="D17" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -968,13 +966,13 @@
         <v>0</v>
       </c>
       <c r="C18" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D18" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -985,13 +983,13 @@
         <v>0</v>
       </c>
       <c r="C19" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="D19" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1002,13 +1000,13 @@
         <v>0</v>
       </c>
       <c r="C20" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D20" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1019,13 +1017,13 @@
         <v>0</v>
       </c>
       <c r="C21" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="D21" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>